<commit_message>
fix: add sede reason column to inquiring report
</commit_message>
<xml_diff>
--- a/reports/inquiring_requests/templates/xlsx/template.xlsx
+++ b/reports/inquiring_requests/templates/xlsx/template.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david.colomer\Documents\CSB\Informes36\custreport\reports\solicitudes_inquiring\templates\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorgelg/git/yssb-devi-reports/reports/inquiring_requests/templates/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84209E4-8041-45F1-9610-6F1F518160F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8725B5-7BD4-F24C-8704-347E2D61F371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36160" yWindow="5520" windowWidth="32080" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$N$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$O$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Request ID</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>Last Change At</t>
+  </si>
+  <si>
+    <t>Sede Reason</t>
   </si>
 </sst>
 </file>
@@ -411,29 +414,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="6" width="17.5703125" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="6" width="17.5" bestFit="1" customWidth="1" outlineLevel="1"/>
     <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="18.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -476,9 +480,12 @@
       <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N1" xr:uid="{4B4C567F-19CC-43F3-A784-B79D65DF0209}"/>
+  <autoFilter ref="A1:O1" xr:uid="{4B4C567F-19CC-43F3-A784-B79D65DF0209}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: add sede reason column to inquiring report (#5)
</commit_message>
<xml_diff>
--- a/reports/inquiring_requests/templates/xlsx/template.xlsx
+++ b/reports/inquiring_requests/templates/xlsx/template.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david.colomer\Documents\CSB\Informes36\custreport\reports\solicitudes_inquiring\templates\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorgelg/git/yssb-devi-reports/reports/inquiring_requests/templates/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84209E4-8041-45F1-9610-6F1F518160F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8725B5-7BD4-F24C-8704-347E2D61F371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36160" yWindow="5520" windowWidth="32080" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$N$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$O$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Request ID</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>Last Change At</t>
+  </si>
+  <si>
+    <t>Sede Reason</t>
   </si>
 </sst>
 </file>
@@ -411,29 +414,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="6" width="17.5703125" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="6" width="17.5" bestFit="1" customWidth="1" outlineLevel="1"/>
     <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="18.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -476,9 +480,12 @@
       <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N1" xr:uid="{4B4C567F-19CC-43F3-A784-B79D65DF0209}"/>
+  <autoFilter ref="A1:O1" xr:uid="{4B4C567F-19CC-43F3-A784-B79D65DF0209}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: add new fields to inquiring report
</commit_message>
<xml_diff>
--- a/reports/inquiring_requests/templates/xlsx/template.xlsx
+++ b/reports/inquiring_requests/templates/xlsx/template.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorgelg/git/yssb-devi-reports/reports/inquiring_requests/templates/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8725B5-7BD4-F24C-8704-347E2D61F371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{506FF24E-FFE0-C74A-9646-1F37ED800472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36160" yWindow="5520" windowWidth="32080" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30760" yWindow="5180" windowWidth="32080" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$O$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$R$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Request ID</t>
   </si>
@@ -68,6 +68,15 @@
   </si>
   <si>
     <t>Sede Reason</t>
+  </si>
+  <si>
+    <t>Sede</t>
+  </si>
+  <si>
+    <t>Postal Address</t>
+  </si>
+  <si>
+    <t>Sales TE EMail</t>
   </si>
 </sst>
 </file>
@@ -414,17 +423,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="2" max="2" width="22" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1" outlineLevel="1"/>
     <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1" outlineLevel="1"/>
     <col min="5" max="6" width="17.5" bestFit="1" customWidth="1" outlineLevel="1"/>
     <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
@@ -434,10 +443,11 @@
     <col min="11" max="12" width="18.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="15.33203125" customWidth="1"/>
+    <col min="18" max="18" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -481,11 +491,20 @@
         <v>12</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O1" xr:uid="{4B4C567F-19CC-43F3-A784-B79D65DF0209}"/>
+  <autoFilter ref="A1:R1" xr:uid="{4B4C567F-19CC-43F3-A784-B79D65DF0209}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: add new fields to inquiring report (#6)
</commit_message>
<xml_diff>
--- a/reports/inquiring_requests/templates/xlsx/template.xlsx
+++ b/reports/inquiring_requests/templates/xlsx/template.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorgelg/git/yssb-devi-reports/reports/inquiring_requests/templates/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8725B5-7BD4-F24C-8704-347E2D61F371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{506FF24E-FFE0-C74A-9646-1F37ED800472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36160" yWindow="5520" windowWidth="32080" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30760" yWindow="5180" windowWidth="32080" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$O$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$R$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Request ID</t>
   </si>
@@ -68,6 +68,15 @@
   </si>
   <si>
     <t>Sede Reason</t>
+  </si>
+  <si>
+    <t>Sede</t>
+  </si>
+  <si>
+    <t>Postal Address</t>
+  </si>
+  <si>
+    <t>Sales TE EMail</t>
   </si>
 </sst>
 </file>
@@ -414,17 +423,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="2" max="2" width="22" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1" outlineLevel="1"/>
     <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1" outlineLevel="1"/>
     <col min="5" max="6" width="17.5" bestFit="1" customWidth="1" outlineLevel="1"/>
     <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
@@ -434,10 +443,11 @@
     <col min="11" max="12" width="18.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="15.33203125" customWidth="1"/>
+    <col min="18" max="18" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -481,11 +491,20 @@
         <v>12</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O1" xr:uid="{4B4C567F-19CC-43F3-A784-B79D65DF0209}"/>
+  <autoFilter ref="A1:R1" xr:uid="{4B4C567F-19CC-43F3-A784-B79D65DF0209}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>